<commit_message>
added private jets apron + ellx hangar stands
</commit_message>
<xml_diff>
--- a/api/data/gates_db.xlsx
+++ b/api/data/gates_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\belux\belux-gate-manager-api\api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA9A7AA-FBF1-4C2B-8E8F-9A0EAFB0430F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB977BB-E3C0-4E84-8EAA-BFD6C126A46F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
+    <workbookView xWindow="21030" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1237" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="689">
   <si>
     <t>505335.23N</t>
   </si>
@@ -3202,6 +3202,15 @@
   </si>
   <si>
     <t>0042914.71E</t>
+  </si>
+  <si>
+    <t>apron-P8</t>
+  </si>
+  <si>
+    <t>MNT1</t>
+  </si>
+  <si>
+    <t>MNT2</t>
   </si>
 </sst>
 </file>
@@ -3637,10 +3646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A74C131-8C0C-4CF6-B99D-A6421F63E231}">
-  <dimension ref="A1:O284"/>
+  <dimension ref="A1:O286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A284" sqref="A284:XFD284"/>
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C291" sqref="C291"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19037,6 +19046,40 @@
         <v>6.1972882396987803</v>
       </c>
     </row>
+    <row r="285" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>426</v>
+      </c>
+      <c r="B285" t="s">
+        <v>686</v>
+      </c>
+      <c r="C285" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="K285">
+        <v>49.617411383833499</v>
+      </c>
+      <c r="O285">
+        <v>6.1998207863052102</v>
+      </c>
+    </row>
+    <row r="286" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>426</v>
+      </c>
+      <c r="B286" t="s">
+        <v>686</v>
+      </c>
+      <c r="C286" s="2" t="s">
+        <v>688</v>
+      </c>
+      <c r="K286">
+        <v>49.617793692219699</v>
+      </c>
+      <c r="O286">
+        <v>6.2009902293549599</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
data fixes + removed trail 0's ELLX
</commit_message>
<xml_diff>
--- a/api/data/gates_db.xlsx
+++ b/api/data/gates_db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\belux\belux-gate-manager-api\api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7279F4E2-DCF1-49E3-A188-BA9017860486}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4CABC5F-F6DB-4C8E-8112-7AEE28C13CB7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -2637,48 +2637,9 @@
     <t>0061310.81E</t>
   </si>
   <si>
-    <t>A02</t>
-  </si>
-  <si>
-    <t>A04</t>
-  </si>
-  <si>
-    <t>A06</t>
-  </si>
-  <si>
-    <t>A08</t>
-  </si>
-  <si>
     <t>A12</t>
   </si>
   <si>
-    <t>B01</t>
-  </si>
-  <si>
-    <t>B02</t>
-  </si>
-  <si>
-    <t>B03</t>
-  </si>
-  <si>
-    <t>B04</t>
-  </si>
-  <si>
-    <t>B05</t>
-  </si>
-  <si>
-    <t>B06</t>
-  </si>
-  <si>
-    <t>B07</t>
-  </si>
-  <si>
-    <t>B08</t>
-  </si>
-  <si>
-    <t>B09</t>
-  </si>
-  <si>
     <t>apron-P1-A-nonshengen</t>
   </si>
   <si>
@@ -3175,6 +3136,45 @@
   </si>
   <si>
     <t>MNT2</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A6</t>
+  </si>
+  <si>
+    <t>A8</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B5</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
+    <t>B7</t>
+  </si>
+  <si>
+    <t>B8</t>
+  </si>
+  <si>
+    <t>B9</t>
   </si>
 </sst>
 </file>
@@ -3612,8 +3612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A74C131-8C0C-4CF6-B99D-A6421F63E231}">
   <dimension ref="A1:O282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B225" sqref="B225"/>
+    <sheetView tabSelected="1" topLeftCell="A193" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C238" sqref="C238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9165,7 +9165,7 @@
         <v>49</v>
       </c>
       <c r="E98" t="s">
-        <v>673</v>
+        <v>660</v>
       </c>
       <c r="F98" t="str">
         <f t="shared" si="17"/>
@@ -14216,10 +14216,10 @@
         <v>426</v>
       </c>
       <c r="B198" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>497</v>
+        <v>664</v>
       </c>
       <c r="D198" t="s">
         <v>427</v>
@@ -14273,10 +14273,10 @@
         <v>426</v>
       </c>
       <c r="B199" t="s">
-        <v>511</v>
+        <v>498</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>498</v>
+        <v>665</v>
       </c>
       <c r="D199" t="s">
         <v>429</v>
@@ -14330,10 +14330,10 @@
         <v>426</v>
       </c>
       <c r="B200" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>499</v>
+        <v>666</v>
       </c>
       <c r="D200" t="s">
         <v>431</v>
@@ -14387,10 +14387,10 @@
         <v>426</v>
       </c>
       <c r="B201" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>500</v>
+        <v>667</v>
       </c>
       <c r="D201" t="s">
         <v>433</v>
@@ -14444,7 +14444,7 @@
         <v>426</v>
       </c>
       <c r="B202" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>435</v>
@@ -14501,10 +14501,10 @@
         <v>426</v>
       </c>
       <c r="B203" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D203" t="s">
         <v>438</v>
@@ -14558,7 +14558,7 @@
         <v>426</v>
       </c>
       <c r="B204" t="s">
-        <v>513</v>
+        <v>500</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>440</v>
@@ -14615,10 +14615,10 @@
         <v>426</v>
       </c>
       <c r="B205" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>502</v>
+        <v>668</v>
       </c>
       <c r="D205" t="s">
         <v>443</v>
@@ -14672,10 +14672,10 @@
         <v>426</v>
       </c>
       <c r="B206" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>503</v>
+        <v>669</v>
       </c>
       <c r="D206" t="s">
         <v>445</v>
@@ -14729,10 +14729,10 @@
         <v>426</v>
       </c>
       <c r="B207" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>504</v>
+        <v>670</v>
       </c>
       <c r="D207" t="s">
         <v>447</v>
@@ -14786,10 +14786,10 @@
         <v>426</v>
       </c>
       <c r="B208" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C208" s="2" t="s">
-        <v>505</v>
+        <v>671</v>
       </c>
       <c r="D208" t="s">
         <v>449</v>
@@ -14843,10 +14843,10 @@
         <v>426</v>
       </c>
       <c r="B209" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>506</v>
+        <v>672</v>
       </c>
       <c r="D209" t="s">
         <v>451</v>
@@ -14900,10 +14900,10 @@
         <v>426</v>
       </c>
       <c r="B210" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>507</v>
+        <v>673</v>
       </c>
       <c r="D210" t="s">
         <v>453</v>
@@ -14957,10 +14957,10 @@
         <v>426</v>
       </c>
       <c r="B211" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>508</v>
+        <v>674</v>
       </c>
       <c r="D211" t="s">
         <v>455</v>
@@ -15014,10 +15014,10 @@
         <v>426</v>
       </c>
       <c r="B212" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>509</v>
+        <v>675</v>
       </c>
       <c r="D212" t="s">
         <v>457</v>
@@ -15071,10 +15071,10 @@
         <v>426</v>
       </c>
       <c r="B213" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>510</v>
+        <v>676</v>
       </c>
       <c r="D213" t="s">
         <v>459</v>
@@ -15128,7 +15128,7 @@
         <v>426</v>
       </c>
       <c r="B214" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="C214" s="2" t="s">
         <v>461</v>
@@ -15185,7 +15185,7 @@
         <v>426</v>
       </c>
       <c r="B215" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>464</v>
@@ -15242,7 +15242,7 @@
         <v>426</v>
       </c>
       <c r="B216" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="C216" s="2" t="s">
         <v>467</v>
@@ -15299,7 +15299,7 @@
         <v>426</v>
       </c>
       <c r="B217" t="s">
-        <v>512</v>
+        <v>499</v>
       </c>
       <c r="C217" s="2" t="s">
         <v>470</v>
@@ -15356,7 +15356,7 @@
         <v>426</v>
       </c>
       <c r="B218" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C218" s="2" t="s">
         <v>473</v>
@@ -15413,7 +15413,7 @@
         <v>426</v>
       </c>
       <c r="B219" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>476</v>
@@ -15470,7 +15470,7 @@
         <v>426</v>
       </c>
       <c r="B220" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C220" s="2" t="s">
         <v>479</v>
@@ -15527,7 +15527,7 @@
         <v>426</v>
       </c>
       <c r="B221" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>482</v>
@@ -15584,7 +15584,7 @@
         <v>426</v>
       </c>
       <c r="B222" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>485</v>
@@ -15641,7 +15641,7 @@
         <v>426</v>
       </c>
       <c r="B223" t="s">
-        <v>515</v>
+        <v>502</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>488</v>
@@ -15698,7 +15698,7 @@
         <v>426</v>
       </c>
       <c r="B224" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="C224" s="2" t="s">
         <v>491</v>
@@ -15755,7 +15755,7 @@
         <v>426</v>
       </c>
       <c r="B225" t="s">
-        <v>516</v>
+        <v>503</v>
       </c>
       <c r="C225" s="2" t="s">
         <v>494</v>
@@ -15812,16 +15812,16 @@
         <v>426</v>
       </c>
       <c r="B226" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>517</v>
+        <v>504</v>
       </c>
       <c r="D226" t="s">
-        <v>518</v>
+        <v>505</v>
       </c>
       <c r="E226" t="s">
-        <v>519</v>
+        <v>506</v>
       </c>
       <c r="F226" t="str">
         <f t="shared" ref="F226:F237" si="58">SUBSTITUTE( SUBSTITUTE(D226,"N",""),",",".")</f>
@@ -15869,16 +15869,16 @@
         <v>426</v>
       </c>
       <c r="B227" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>520</v>
+        <v>507</v>
       </c>
       <c r="D227" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="E227" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="F227" t="str">
         <f t="shared" si="58"/>
@@ -15926,16 +15926,16 @@
         <v>426</v>
       </c>
       <c r="B228" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="D228" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="E228" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="F228" t="str">
         <f t="shared" si="58"/>
@@ -15983,16 +15983,16 @@
         <v>426</v>
       </c>
       <c r="B229" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="D229" t="s">
-        <v>527</v>
+        <v>514</v>
       </c>
       <c r="E229" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
       <c r="F229" t="str">
         <f t="shared" si="58"/>
@@ -16040,16 +16040,16 @@
         <v>426</v>
       </c>
       <c r="B230" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C230" s="2" t="s">
-        <v>529</v>
+        <v>516</v>
       </c>
       <c r="D230" t="s">
-        <v>530</v>
+        <v>517</v>
       </c>
       <c r="E230" t="s">
-        <v>531</v>
+        <v>518</v>
       </c>
       <c r="F230" t="str">
         <f t="shared" si="58"/>
@@ -16097,16 +16097,16 @@
         <v>426</v>
       </c>
       <c r="B231" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C231" s="2" t="s">
-        <v>532</v>
+        <v>519</v>
       </c>
       <c r="D231" t="s">
-        <v>533</v>
+        <v>520</v>
       </c>
       <c r="E231" t="s">
-        <v>534</v>
+        <v>521</v>
       </c>
       <c r="F231" t="str">
         <f t="shared" si="58"/>
@@ -16154,16 +16154,16 @@
         <v>426</v>
       </c>
       <c r="B232" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C232" s="2" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="D232" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="E232" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="F232" t="str">
         <f t="shared" si="58"/>
@@ -16211,16 +16211,16 @@
         <v>426</v>
       </c>
       <c r="B233" t="s">
-        <v>553</v>
+        <v>540</v>
       </c>
       <c r="C233" s="2" t="s">
-        <v>538</v>
+        <v>525</v>
       </c>
       <c r="D233" t="s">
-        <v>539</v>
+        <v>526</v>
       </c>
       <c r="E233" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="F233" t="str">
         <f t="shared" si="58"/>
@@ -16268,16 +16268,16 @@
         <v>426</v>
       </c>
       <c r="B234" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="C234" s="2" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
       <c r="D234" t="s">
-        <v>542</v>
+        <v>529</v>
       </c>
       <c r="E234" t="s">
-        <v>543</v>
+        <v>530</v>
       </c>
       <c r="F234" t="str">
         <f t="shared" si="58"/>
@@ -16325,16 +16325,16 @@
         <v>426</v>
       </c>
       <c r="B235" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="C235" s="2" t="s">
-        <v>544</v>
+        <v>531</v>
       </c>
       <c r="D235" t="s">
-        <v>545</v>
+        <v>532</v>
       </c>
       <c r="E235" t="s">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="F235" t="str">
         <f t="shared" si="58"/>
@@ -16382,16 +16382,16 @@
         <v>426</v>
       </c>
       <c r="B236" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="C236" s="2" t="s">
-        <v>547</v>
+        <v>534</v>
       </c>
       <c r="D236" t="s">
-        <v>548</v>
+        <v>535</v>
       </c>
       <c r="E236" t="s">
-        <v>549</v>
+        <v>536</v>
       </c>
       <c r="F236" t="str">
         <f t="shared" si="58"/>
@@ -16439,16 +16439,16 @@
         <v>426</v>
       </c>
       <c r="B237" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="C237" s="2" t="s">
-        <v>550</v>
+        <v>537</v>
       </c>
       <c r="D237" t="s">
-        <v>551</v>
+        <v>538</v>
       </c>
       <c r="E237" t="s">
-        <v>552</v>
+        <v>539</v>
       </c>
       <c r="F237" t="str">
         <f t="shared" si="58"/>
@@ -16496,16 +16496,16 @@
         <v>426</v>
       </c>
       <c r="B238" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C238" s="2" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
       <c r="D238" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="E238" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="F238" t="str">
         <f t="shared" ref="F238:F276" si="68">SUBSTITUTE( SUBSTITUTE(D238,"N",""),",",".")</f>
@@ -16553,16 +16553,16 @@
         <v>426</v>
       </c>
       <c r="B239" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C239" s="2" t="s">
-        <v>667</v>
+        <v>654</v>
       </c>
       <c r="D239" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="E239" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="F239" t="str">
         <f t="shared" si="68"/>
@@ -16610,16 +16610,16 @@
         <v>426</v>
       </c>
       <c r="B240" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C240" s="2" t="s">
-        <v>668</v>
+        <v>655</v>
       </c>
       <c r="D240" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="E240" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="F240" t="str">
         <f t="shared" si="68"/>
@@ -16667,16 +16667,16 @@
         <v>426</v>
       </c>
       <c r="B241" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C241" s="2" t="s">
-        <v>669</v>
+        <v>656</v>
       </c>
       <c r="D241" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="E241" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="F241" t="str">
         <f t="shared" si="68"/>
@@ -16724,16 +16724,16 @@
         <v>426</v>
       </c>
       <c r="B242" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C242" s="2" t="s">
-        <v>670</v>
+        <v>657</v>
       </c>
       <c r="D242" t="s">
-        <v>563</v>
+        <v>550</v>
       </c>
       <c r="E242" t="s">
-        <v>564</v>
+        <v>551</v>
       </c>
       <c r="F242" t="str">
         <f t="shared" si="68"/>
@@ -16781,16 +16781,16 @@
         <v>426</v>
       </c>
       <c r="B243" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C243" s="2" t="s">
-        <v>565</v>
+        <v>552</v>
       </c>
       <c r="D243" t="s">
-        <v>566</v>
+        <v>553</v>
       </c>
       <c r="E243" t="s">
-        <v>567</v>
+        <v>554</v>
       </c>
       <c r="F243" t="str">
         <f t="shared" si="68"/>
@@ -16838,16 +16838,16 @@
         <v>426</v>
       </c>
       <c r="B244" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C244" s="2" t="s">
-        <v>568</v>
+        <v>555</v>
       </c>
       <c r="D244" t="s">
-        <v>569</v>
+        <v>556</v>
       </c>
       <c r="E244" t="s">
-        <v>570</v>
+        <v>557</v>
       </c>
       <c r="F244" t="str">
         <f t="shared" si="68"/>
@@ -16895,16 +16895,16 @@
         <v>426</v>
       </c>
       <c r="B245" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C245" s="2" t="s">
-        <v>571</v>
+        <v>558</v>
       </c>
       <c r="D245" t="s">
-        <v>572</v>
+        <v>559</v>
       </c>
       <c r="E245" t="s">
-        <v>573</v>
+        <v>560</v>
       </c>
       <c r="F245" t="str">
         <f t="shared" si="68"/>
@@ -16952,16 +16952,16 @@
         <v>426</v>
       </c>
       <c r="B246" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C246" s="2" t="s">
-        <v>574</v>
+        <v>561</v>
       </c>
       <c r="D246" t="s">
-        <v>575</v>
+        <v>562</v>
       </c>
       <c r="E246" t="s">
-        <v>576</v>
+        <v>563</v>
       </c>
       <c r="F246" t="str">
         <f t="shared" si="68"/>
@@ -17009,16 +17009,16 @@
         <v>426</v>
       </c>
       <c r="B247" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C247" s="2" t="s">
-        <v>577</v>
+        <v>564</v>
       </c>
       <c r="D247" t="s">
-        <v>578</v>
+        <v>565</v>
       </c>
       <c r="E247" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="F247" t="str">
         <f t="shared" si="68"/>
@@ -17066,16 +17066,16 @@
         <v>426</v>
       </c>
       <c r="B248" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C248" s="2" t="s">
-        <v>580</v>
+        <v>567</v>
       </c>
       <c r="D248" t="s">
-        <v>581</v>
+        <v>568</v>
       </c>
       <c r="E248" t="s">
-        <v>582</v>
+        <v>569</v>
       </c>
       <c r="F248" t="str">
         <f t="shared" si="68"/>
@@ -17123,16 +17123,16 @@
         <v>426</v>
       </c>
       <c r="B249" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C249" s="2" t="s">
-        <v>583</v>
+        <v>570</v>
       </c>
       <c r="D249" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="E249" t="s">
-        <v>585</v>
+        <v>572</v>
       </c>
       <c r="F249" t="str">
         <f t="shared" si="68"/>
@@ -17180,16 +17180,16 @@
         <v>426</v>
       </c>
       <c r="B250" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C250" s="2" t="s">
-        <v>586</v>
+        <v>573</v>
       </c>
       <c r="D250" t="s">
-        <v>587</v>
+        <v>574</v>
       </c>
       <c r="E250" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
       <c r="F250" t="str">
         <f t="shared" si="68"/>
@@ -17237,16 +17237,16 @@
         <v>426</v>
       </c>
       <c r="B251" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C251" s="2" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="D251" t="s">
-        <v>590</v>
+        <v>577</v>
       </c>
       <c r="E251" t="s">
-        <v>591</v>
+        <v>578</v>
       </c>
       <c r="F251" t="str">
         <f t="shared" si="68"/>
@@ -17294,16 +17294,16 @@
         <v>426</v>
       </c>
       <c r="B252" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>592</v>
+        <v>579</v>
       </c>
       <c r="D252" t="s">
-        <v>593</v>
+        <v>580</v>
       </c>
       <c r="E252" t="s">
-        <v>594</v>
+        <v>581</v>
       </c>
       <c r="F252" t="str">
         <f t="shared" si="68"/>
@@ -17351,16 +17351,16 @@
         <v>426</v>
       </c>
       <c r="B253" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C253" s="2" t="s">
-        <v>595</v>
+        <v>582</v>
       </c>
       <c r="D253" t="s">
-        <v>596</v>
+        <v>583</v>
       </c>
       <c r="E253" t="s">
-        <v>597</v>
+        <v>584</v>
       </c>
       <c r="F253" t="str">
         <f t="shared" si="68"/>
@@ -17408,16 +17408,16 @@
         <v>426</v>
       </c>
       <c r="B254" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C254" s="2" t="s">
-        <v>598</v>
+        <v>585</v>
       </c>
       <c r="D254" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="E254" t="s">
-        <v>599</v>
+        <v>586</v>
       </c>
       <c r="F254" t="str">
         <f t="shared" si="68"/>
@@ -17465,16 +17465,16 @@
         <v>426</v>
       </c>
       <c r="B255" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C255" s="2" t="s">
-        <v>600</v>
+        <v>587</v>
       </c>
       <c r="D255" t="s">
-        <v>601</v>
+        <v>588</v>
       </c>
       <c r="E255" t="s">
-        <v>602</v>
+        <v>589</v>
       </c>
       <c r="F255" t="str">
         <f t="shared" si="68"/>
@@ -17522,16 +17522,16 @@
         <v>426</v>
       </c>
       <c r="B256" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C256" s="2" t="s">
-        <v>603</v>
+        <v>590</v>
       </c>
       <c r="D256" t="s">
-        <v>604</v>
+        <v>591</v>
       </c>
       <c r="E256" t="s">
-        <v>605</v>
+        <v>592</v>
       </c>
       <c r="F256" t="str">
         <f t="shared" si="68"/>
@@ -17579,16 +17579,16 @@
         <v>426</v>
       </c>
       <c r="B257" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C257" s="2" t="s">
-        <v>606</v>
+        <v>593</v>
       </c>
       <c r="D257" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="E257" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
       <c r="F257" t="str">
         <f t="shared" si="68"/>
@@ -17636,16 +17636,16 @@
         <v>426</v>
       </c>
       <c r="B258" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C258" s="2" t="s">
-        <v>609</v>
+        <v>596</v>
       </c>
       <c r="D258" t="s">
-        <v>610</v>
+        <v>597</v>
       </c>
       <c r="E258" t="s">
-        <v>611</v>
+        <v>598</v>
       </c>
       <c r="F258" t="str">
         <f t="shared" si="68"/>
@@ -17693,16 +17693,16 @@
         <v>426</v>
       </c>
       <c r="B259" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C259" s="2" t="s">
-        <v>612</v>
+        <v>599</v>
       </c>
       <c r="D259" t="s">
-        <v>613</v>
+        <v>600</v>
       </c>
       <c r="E259" t="s">
-        <v>614</v>
+        <v>601</v>
       </c>
       <c r="F259" t="str">
         <f t="shared" si="68"/>
@@ -17750,16 +17750,16 @@
         <v>426</v>
       </c>
       <c r="B260" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C260" s="2" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
       <c r="D260" t="s">
-        <v>616</v>
+        <v>603</v>
       </c>
       <c r="E260" t="s">
-        <v>617</v>
+        <v>604</v>
       </c>
       <c r="F260" t="str">
         <f t="shared" si="68"/>
@@ -17807,16 +17807,16 @@
         <v>426</v>
       </c>
       <c r="B261" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>618</v>
+        <v>605</v>
       </c>
       <c r="D261" t="s">
-        <v>619</v>
+        <v>606</v>
       </c>
       <c r="E261" t="s">
-        <v>620</v>
+        <v>607</v>
       </c>
       <c r="F261" t="str">
         <f t="shared" si="68"/>
@@ -17864,16 +17864,16 @@
         <v>426</v>
       </c>
       <c r="B262" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C262" s="2" t="s">
-        <v>621</v>
+        <v>608</v>
       </c>
       <c r="D262" t="s">
-        <v>622</v>
+        <v>609</v>
       </c>
       <c r="E262" t="s">
-        <v>623</v>
+        <v>610</v>
       </c>
       <c r="F262" t="str">
         <f t="shared" si="68"/>
@@ -17921,16 +17921,16 @@
         <v>426</v>
       </c>
       <c r="B263" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C263" s="2" t="s">
-        <v>624</v>
+        <v>611</v>
       </c>
       <c r="D263" t="s">
-        <v>625</v>
+        <v>612</v>
       </c>
       <c r="E263" t="s">
-        <v>626</v>
+        <v>613</v>
       </c>
       <c r="F263" t="str">
         <f t="shared" si="68"/>
@@ -17978,16 +17978,16 @@
         <v>426</v>
       </c>
       <c r="B264" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C264" s="2" t="s">
-        <v>627</v>
+        <v>614</v>
       </c>
       <c r="D264" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="E264" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
       <c r="F264" t="str">
         <f t="shared" si="68"/>
@@ -18035,16 +18035,16 @@
         <v>426</v>
       </c>
       <c r="B265" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C265" s="2" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
       <c r="D265" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
       <c r="E265" t="s">
-        <v>632</v>
+        <v>619</v>
       </c>
       <c r="F265" t="str">
         <f t="shared" si="68"/>
@@ -18092,16 +18092,16 @@
         <v>426</v>
       </c>
       <c r="B266" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C266" s="2" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
       <c r="D266" t="s">
-        <v>634</v>
+        <v>621</v>
       </c>
       <c r="E266" t="s">
-        <v>635</v>
+        <v>622</v>
       </c>
       <c r="F266" t="str">
         <f t="shared" si="68"/>
@@ -18149,16 +18149,16 @@
         <v>426</v>
       </c>
       <c r="B267" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C267" s="2" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
       <c r="D267" t="s">
-        <v>637</v>
+        <v>624</v>
       </c>
       <c r="E267" t="s">
-        <v>638</v>
+        <v>625</v>
       </c>
       <c r="F267" t="str">
         <f t="shared" si="68"/>
@@ -18206,16 +18206,16 @@
         <v>426</v>
       </c>
       <c r="B268" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C268" s="2" t="s">
-        <v>639</v>
+        <v>626</v>
       </c>
       <c r="D268" t="s">
-        <v>640</v>
+        <v>627</v>
       </c>
       <c r="E268" t="s">
-        <v>641</v>
+        <v>628</v>
       </c>
       <c r="F268" t="str">
         <f t="shared" si="68"/>
@@ -18263,16 +18263,16 @@
         <v>426</v>
       </c>
       <c r="B269" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C269" s="2" t="s">
-        <v>642</v>
+        <v>629</v>
       </c>
       <c r="D269" t="s">
-        <v>643</v>
+        <v>630</v>
       </c>
       <c r="E269" t="s">
-        <v>644</v>
+        <v>631</v>
       </c>
       <c r="F269" t="str">
         <f t="shared" si="68"/>
@@ -18320,16 +18320,16 @@
         <v>426</v>
       </c>
       <c r="B270" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C270" s="2" t="s">
-        <v>645</v>
+        <v>632</v>
       </c>
       <c r="D270" t="s">
-        <v>646</v>
+        <v>633</v>
       </c>
       <c r="E270" t="s">
-        <v>647</v>
+        <v>634</v>
       </c>
       <c r="F270" t="str">
         <f t="shared" si="68"/>
@@ -18377,16 +18377,16 @@
         <v>426</v>
       </c>
       <c r="B271" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C271" s="2" t="s">
-        <v>648</v>
+        <v>635</v>
       </c>
       <c r="D271" t="s">
-        <v>649</v>
+        <v>636</v>
       </c>
       <c r="E271" t="s">
-        <v>650</v>
+        <v>637</v>
       </c>
       <c r="F271" t="str">
         <f t="shared" si="68"/>
@@ -18434,16 +18434,16 @@
         <v>426</v>
       </c>
       <c r="B272" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C272" s="2" t="s">
-        <v>651</v>
+        <v>638</v>
       </c>
       <c r="D272" t="s">
-        <v>652</v>
+        <v>639</v>
       </c>
       <c r="E272" t="s">
-        <v>653</v>
+        <v>640</v>
       </c>
       <c r="F272" t="str">
         <f t="shared" si="68"/>
@@ -18491,16 +18491,16 @@
         <v>426</v>
       </c>
       <c r="B273" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C273" s="2" t="s">
-        <v>654</v>
+        <v>641</v>
       </c>
       <c r="D273" t="s">
-        <v>655</v>
+        <v>642</v>
       </c>
       <c r="E273" t="s">
-        <v>656</v>
+        <v>643</v>
       </c>
       <c r="F273" t="str">
         <f t="shared" si="68"/>
@@ -18548,16 +18548,16 @@
         <v>426</v>
       </c>
       <c r="B274" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C274" s="2" t="s">
-        <v>657</v>
+        <v>644</v>
       </c>
       <c r="D274" t="s">
-        <v>658</v>
+        <v>645</v>
       </c>
       <c r="E274" t="s">
-        <v>659</v>
+        <v>646</v>
       </c>
       <c r="F274" t="str">
         <f t="shared" si="68"/>
@@ -18605,16 +18605,16 @@
         <v>426</v>
       </c>
       <c r="B275" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C275" s="2" t="s">
-        <v>660</v>
+        <v>647</v>
       </c>
       <c r="D275" t="s">
-        <v>661</v>
+        <v>648</v>
       </c>
       <c r="E275" t="s">
-        <v>662</v>
+        <v>649</v>
       </c>
       <c r="F275" t="str">
         <f t="shared" si="68"/>
@@ -18662,16 +18662,16 @@
         <v>426</v>
       </c>
       <c r="B276" t="s">
-        <v>671</v>
+        <v>658</v>
       </c>
       <c r="C276" s="2" t="s">
-        <v>663</v>
+        <v>650</v>
       </c>
       <c r="D276" t="s">
-        <v>664</v>
+        <v>651</v>
       </c>
       <c r="E276" t="s">
-        <v>665</v>
+        <v>652</v>
       </c>
       <c r="F276" t="str">
         <f t="shared" si="68"/>
@@ -18719,7 +18719,7 @@
         <v>426</v>
       </c>
       <c r="B277" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>414</v>
@@ -18736,7 +18736,7 @@
         <v>426</v>
       </c>
       <c r="B278" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>415</v>
@@ -18753,7 +18753,7 @@
         <v>426</v>
       </c>
       <c r="B279" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>416</v>
@@ -18770,7 +18770,7 @@
         <v>426</v>
       </c>
       <c r="B280" t="s">
-        <v>672</v>
+        <v>659</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>417</v>
@@ -18787,10 +18787,10 @@
         <v>426</v>
       </c>
       <c r="B281" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="C281" s="2" t="s">
-        <v>675</v>
+        <v>662</v>
       </c>
       <c r="K281">
         <v>49.617411383833499</v>
@@ -18804,10 +18804,10 @@
         <v>426</v>
       </c>
       <c r="B282" t="s">
-        <v>674</v>
+        <v>661</v>
       </c>
       <c r="C282" s="2" t="s">
-        <v>676</v>
+        <v>663</v>
       </c>
       <c r="K282">
         <v>49.617793692219699</v>

</xml_diff>

<commit_message>
removed new north gates EBLG
</commit_message>
<xml_diff>
--- a/api/data/gates_db.xlsx
+++ b/api/data/gates_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\belux\belux-gate-manager-api\api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A11618F5-F81F-47F0-B4F6-A8E3F2AF3AC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06334332-78DA-45EF-B83C-DA2D7A5E8BCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="1050" windowWidth="21600" windowHeight="11385" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
+    <workbookView xWindow="7200" yWindow="1050" windowWidth="21600" windowHeight="11385" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="1290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="1291">
   <si>
     <t>505335.23N</t>
   </si>
@@ -7001,6 +7001,9 @@
   </si>
   <si>
     <t>apron-2-overflow</t>
+  </si>
+  <si>
+    <t>apron-north-new</t>
   </si>
 </sst>
 </file>
@@ -7460,8 +7463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A74C131-8C0C-4CF6-B99D-A6421F63E231}">
   <dimension ref="A1:O479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A417" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B435" sqref="B435"/>
+    <sheetView tabSelected="1" topLeftCell="A378" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B393" sqref="B393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28930,7 +28933,7 @@
         <v>857</v>
       </c>
       <c r="B392" t="s">
-        <v>904</v>
+        <v>1290</v>
       </c>
       <c r="C392" s="22">
         <v>130</v>
@@ -28986,8 +28989,8 @@
       <c r="A393" t="s">
         <v>857</v>
       </c>
-      <c r="B393" t="s">
-        <v>904</v>
+      <c r="B393" s="29" t="s">
+        <v>1290</v>
       </c>
       <c r="C393" s="22">
         <v>132</v>
@@ -29043,8 +29046,8 @@
       <c r="A394" t="s">
         <v>857</v>
       </c>
-      <c r="B394" t="s">
-        <v>904</v>
+      <c r="B394" s="29" t="s">
+        <v>1290</v>
       </c>
       <c r="C394" s="22">
         <v>134</v>
@@ -29100,8 +29103,8 @@
       <c r="A395" t="s">
         <v>857</v>
       </c>
-      <c r="B395" t="s">
-        <v>904</v>
+      <c r="B395" s="29" t="s">
+        <v>1290</v>
       </c>
       <c r="C395" s="22">
         <v>136</v>
@@ -29157,8 +29160,8 @@
       <c r="A396" t="s">
         <v>857</v>
       </c>
-      <c r="B396" t="s">
-        <v>904</v>
+      <c r="B396" s="29" t="s">
+        <v>1290</v>
       </c>
       <c r="C396" s="22">
         <v>138</v>
@@ -29214,8 +29217,8 @@
       <c r="A397" t="s">
         <v>857</v>
       </c>
-      <c r="B397" t="s">
-        <v>904</v>
+      <c r="B397" s="29" t="s">
+        <v>1290</v>
       </c>
       <c r="C397" s="22">
         <v>140</v>

</xml_diff>

<commit_message>
fixed duplicate stands in EBOS
</commit_message>
<xml_diff>
--- a/api/data/gates_db.xlsx
+++ b/api/data/gates_db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\belux\belux-gate-manager-api\api\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06334332-78DA-45EF-B83C-DA2D7A5E8BCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870324B3-CE22-46E5-8AF4-226DD4CD1046}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="1050" windowWidth="21600" windowHeight="11385" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A18B69D9-28ED-47D3-8556-C314F1DB8CFD}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2222" uniqueCount="1291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="1303">
   <si>
     <t>505335.23N</t>
   </si>
@@ -7004,6 +7004,42 @@
   </si>
   <si>
     <t>apron-north-new</t>
+  </si>
+  <si>
+    <t>P1-1</t>
+  </si>
+  <si>
+    <t>P1-2</t>
+  </si>
+  <si>
+    <t>P1-3</t>
+  </si>
+  <si>
+    <t>P1-4</t>
+  </si>
+  <si>
+    <t>P1-5</t>
+  </si>
+  <si>
+    <t>P1-6</t>
+  </si>
+  <si>
+    <t>P2-1</t>
+  </si>
+  <si>
+    <t>P2-2</t>
+  </si>
+  <si>
+    <t>P2-3</t>
+  </si>
+  <si>
+    <t>P2-4</t>
+  </si>
+  <si>
+    <t>P2-5</t>
+  </si>
+  <si>
+    <t>P2-6</t>
   </si>
 </sst>
 </file>
@@ -7463,8 +7499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A74C131-8C0C-4CF6-B99D-A6421F63E231}">
   <dimension ref="A1:O479"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A378" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B393" sqref="B393"/>
+    <sheetView tabSelected="1" topLeftCell="A417" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C431" sqref="C431"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30439,8 +30475,8 @@
       <c r="B424" s="30" t="s">
         <v>938</v>
       </c>
-      <c r="C424" s="28">
-        <v>1</v>
+      <c r="C424" s="28" t="s">
+        <v>1291</v>
       </c>
       <c r="D424" s="30" t="s">
         <v>1040</v>
@@ -30486,8 +30522,8 @@
       <c r="B425" s="30" t="s">
         <v>938</v>
       </c>
-      <c r="C425" s="28">
-        <v>2</v>
+      <c r="C425" s="28" t="s">
+        <v>1292</v>
       </c>
       <c r="D425" s="30" t="s">
         <v>1044</v>
@@ -30533,8 +30569,8 @@
       <c r="B426" s="30" t="s">
         <v>938</v>
       </c>
-      <c r="C426" s="28">
-        <v>3</v>
+      <c r="C426" s="28" t="s">
+        <v>1293</v>
       </c>
       <c r="D426" s="30" t="s">
         <v>1048</v>
@@ -30580,8 +30616,8 @@
       <c r="B427" s="30" t="s">
         <v>938</v>
       </c>
-      <c r="C427" s="28">
-        <v>4</v>
+      <c r="C427" s="28" t="s">
+        <v>1294</v>
       </c>
       <c r="D427" s="30" t="s">
         <v>1052</v>
@@ -30627,8 +30663,8 @@
       <c r="B428" s="30" t="s">
         <v>938</v>
       </c>
-      <c r="C428" s="28">
-        <v>5</v>
+      <c r="C428" s="28" t="s">
+        <v>1295</v>
       </c>
       <c r="D428" s="30" t="s">
         <v>1056</v>
@@ -30674,8 +30710,8 @@
       <c r="B429" s="30" t="s">
         <v>938</v>
       </c>
-      <c r="C429" s="28">
-        <v>6</v>
+      <c r="C429" s="28" t="s">
+        <v>1296</v>
       </c>
       <c r="D429" s="30" t="s">
         <v>1060</v>
@@ -30721,8 +30757,8 @@
       <c r="B430" s="30" t="s">
         <v>983</v>
       </c>
-      <c r="C430" s="28">
-        <v>1</v>
+      <c r="C430" s="28" t="s">
+        <v>1297</v>
       </c>
       <c r="D430" s="30" t="s">
         <v>1064</v>
@@ -30768,8 +30804,8 @@
       <c r="B431" s="30" t="s">
         <v>983</v>
       </c>
-      <c r="C431" s="28">
-        <v>2</v>
+      <c r="C431" s="28" t="s">
+        <v>1298</v>
       </c>
       <c r="D431" s="30" t="s">
         <v>1068</v>
@@ -30815,8 +30851,8 @@
       <c r="B432" s="30" t="s">
         <v>983</v>
       </c>
-      <c r="C432" s="28">
-        <v>3</v>
+      <c r="C432" s="28" t="s">
+        <v>1299</v>
       </c>
       <c r="D432" s="30" t="s">
         <v>1072</v>
@@ -30862,8 +30898,8 @@
       <c r="B433" s="30" t="s">
         <v>983</v>
       </c>
-      <c r="C433" s="28">
-        <v>4</v>
+      <c r="C433" s="28" t="s">
+        <v>1300</v>
       </c>
       <c r="D433" s="30" t="s">
         <v>1076</v>
@@ -30909,8 +30945,8 @@
       <c r="B434" s="30" t="s">
         <v>1287</v>
       </c>
-      <c r="C434" s="28">
-        <v>5</v>
+      <c r="C434" s="28" t="s">
+        <v>1301</v>
       </c>
       <c r="D434" s="30" t="s">
         <v>1080</v>
@@ -30956,8 +30992,8 @@
       <c r="B435" s="30" t="s">
         <v>1287</v>
       </c>
-      <c r="C435" s="28">
-        <v>6</v>
+      <c r="C435" s="28" t="s">
+        <v>1302</v>
       </c>
       <c r="D435" s="30" t="s">
         <v>1084</v>

</xml_diff>